<commit_message>
2nd pass HIT sample added
</commit_message>
<xml_diff>
--- a/data/QC_Input Sample.xlsx
+++ b/data/QC_Input Sample.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samaydhawan/Downloads/nets213/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="19940" windowHeight="9160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="120">
   <si>
     <t>Truck Name</t>
   </si>
@@ -352,16 +362,48 @@
   </si>
   <si>
     <t>Xlarge regular</t>
+  </si>
+  <si>
+    <t>URL1</t>
+  </si>
+  <si>
+    <t>URL2</t>
+  </si>
+  <si>
+    <t>https://dl.dropboxusercontent.com/u/17481094/12foodtruck_1.jpg</t>
+  </si>
+  <si>
+    <t>https://dl.dropboxusercontent.com/u/17481094/12foodtruck_2.JPG</t>
+  </si>
+  <si>
+    <t>https://dl.dropboxusercontent.com/u/17481094/10foodtruck_1.JPG</t>
+  </si>
+  <si>
+    <t>https://dl.dropboxusercontent.com/u/17481094/10foodtruck_2.JPG</t>
+  </si>
+  <si>
+    <t>Food Item 26</t>
+  </si>
+  <si>
+    <t>Food Item 26 Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -384,13 +426,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,7 +491,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -481,7 +526,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -690,70 +735,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB10"/>
+  <dimension ref="A1:BD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BD4" sqref="BD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="58.6640625" customWidth="1"/>
+    <col min="4" max="4" width="59.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -761,94 +809,94 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
       </c>
       <c r="AG1" t="s">
         <v>29</v>
@@ -916,70 +964,76 @@
       <c r="BB1" t="s">
         <v>101</v>
       </c>
+      <c r="BC1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>915789456</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>42</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>3.5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
         <v>44</v>
       </c>
-      <c r="H2">
-        <v>4.5</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2">
+        <v>4.5</v>
+      </c>
+      <c r="K2" t="s">
         <v>45</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>46</v>
       </c>
-      <c r="L2">
-        <v>4</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2" t="s">
         <v>47</v>
       </c>
-      <c r="N2">
-        <v>4.5</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2">
+        <v>4.5</v>
+      </c>
+      <c r="Q2" t="s">
         <v>49</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>5.5</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>48</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>10</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>50</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>917815835</v>
       </c>
@@ -987,91 +1041,97 @@
         <v>51</v>
       </c>
       <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" t="s">
         <v>103</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3">
         <v>3</v>
       </c>
       <c r="I3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
         <v>106</v>
       </c>
-      <c r="J3">
-        <v>5</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3" t="s">
         <v>56</v>
       </c>
-      <c r="L3">
-        <v>5</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
         <v>57</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>3</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>58</v>
-      </c>
-      <c r="P3">
-        <v>6</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>59</v>
       </c>
       <c r="R3">
         <v>6</v>
       </c>
       <c r="S3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T3">
         <v>6</v>
       </c>
       <c r="U3" t="s">
+        <v>60</v>
+      </c>
+      <c r="V3">
+        <v>6</v>
+      </c>
+      <c r="W3" t="s">
         <v>61</v>
       </c>
-      <c r="V3">
-        <v>5</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="X3">
+        <v>5</v>
+      </c>
+      <c r="Y3" t="s">
         <v>62</v>
-      </c>
-      <c r="X3">
-        <v>3</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>63</v>
       </c>
       <c r="Z3">
         <v>3</v>
       </c>
       <c r="AA3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB3">
+        <v>3</v>
+      </c>
+      <c r="AC3" t="s">
         <v>64</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <v>6</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AE3" t="s">
         <v>65</v>
       </c>
-      <c r="AD3">
+      <c r="AF3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>992145378</v>
       </c>
@@ -1079,281 +1139,287 @@
         <v>66</v>
       </c>
       <c r="C4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
         <v>67</v>
       </c>
-      <c r="D4">
-        <v>4.5</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4">
+        <v>4.5</v>
+      </c>
+      <c r="G4" t="s">
         <v>68</v>
       </c>
-      <c r="F4">
-        <v>4.5</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4">
+        <v>4.5</v>
+      </c>
+      <c r="I4" t="s">
         <v>69</v>
       </c>
-      <c r="H4">
-        <v>4.5</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4">
+        <v>4.5</v>
+      </c>
+      <c r="K4" t="s">
         <v>70</v>
       </c>
-      <c r="J4">
-        <v>4.5</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="L4">
+        <v>4.5</v>
+      </c>
+      <c r="M4" t="s">
         <v>71</v>
       </c>
-      <c r="L4">
-        <v>4.5</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="N4">
+        <v>4.5</v>
+      </c>
+      <c r="O4" t="s">
         <v>72</v>
       </c>
-      <c r="N4">
-        <v>5</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="P4">
+        <v>5</v>
+      </c>
+      <c r="Q4" t="s">
         <v>73</v>
       </c>
-      <c r="P4">
-        <v>5</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4" t="s">
         <v>74</v>
       </c>
-      <c r="R4">
-        <v>4</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="T4">
+        <v>4</v>
+      </c>
+      <c r="U4" t="s">
         <v>75</v>
       </c>
-      <c r="T4">
-        <v>4</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="V4">
+        <v>4</v>
+      </c>
+      <c r="W4" t="s">
         <v>76</v>
       </c>
-      <c r="V4">
-        <v>4</v>
-      </c>
-      <c r="W4" t="s">
+      <c r="X4">
+        <v>4</v>
+      </c>
+      <c r="Y4" t="s">
         <v>77</v>
       </c>
-      <c r="X4">
-        <v>4</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="Z4">
+        <v>4</v>
+      </c>
+      <c r="AA4" t="s">
         <v>78</v>
       </c>
-      <c r="Z4">
-        <v>4</v>
-      </c>
-      <c r="AA4" t="s">
+      <c r="AB4">
+        <v>4</v>
+      </c>
+      <c r="AC4" t="s">
         <v>79</v>
       </c>
-      <c r="AB4">
-        <v>4.5</v>
-      </c>
-      <c r="AC4" t="s">
+      <c r="AD4">
+        <v>4.5</v>
+      </c>
+      <c r="AE4" t="s">
         <v>80</v>
       </c>
-      <c r="AD4">
-        <v>5</v>
-      </c>
-      <c r="AE4" t="s">
+      <c r="AF4">
+        <v>5</v>
+      </c>
+      <c r="AG4" t="s">
         <v>81</v>
       </c>
-      <c r="AF4">
-        <v>5</v>
-      </c>
-      <c r="AG4" t="s">
+      <c r="AH4">
+        <v>5</v>
+      </c>
+      <c r="AI4" t="s">
         <v>82</v>
       </c>
-      <c r="AH4">
-        <v>5</v>
-      </c>
-      <c r="AI4" t="s">
+      <c r="AJ4">
+        <v>5</v>
+      </c>
+      <c r="AK4" t="s">
         <v>83</v>
       </c>
-      <c r="AJ4">
-        <v>5</v>
-      </c>
-      <c r="AK4" t="s">
+      <c r="AL4">
+        <v>5</v>
+      </c>
+      <c r="AM4" t="s">
         <v>84</v>
       </c>
-      <c r="AL4">
-        <v>5</v>
-      </c>
-      <c r="AM4" t="s">
+      <c r="AN4">
+        <v>5</v>
+      </c>
+      <c r="AO4" t="s">
         <v>85</v>
       </c>
-      <c r="AN4">
-        <v>5</v>
-      </c>
-      <c r="AO4" t="s">
+      <c r="AP4">
+        <v>5</v>
+      </c>
+      <c r="AQ4" t="s">
         <v>86</v>
       </c>
-      <c r="AP4">
-        <v>5</v>
-      </c>
-      <c r="AQ4" t="s">
+      <c r="AR4">
+        <v>5</v>
+      </c>
+      <c r="AS4" t="s">
         <v>87</v>
       </c>
-      <c r="AR4">
-        <v>5</v>
-      </c>
-      <c r="AS4" t="s">
+      <c r="AT4">
+        <v>5</v>
+      </c>
+      <c r="AU4" t="s">
         <v>88</v>
       </c>
-      <c r="AT4">
-        <v>5</v>
-      </c>
-      <c r="AU4" t="s">
+      <c r="AV4">
+        <v>5</v>
+      </c>
+      <c r="AW4" t="s">
         <v>89</v>
       </c>
-      <c r="AV4">
-        <v>5</v>
-      </c>
-      <c r="AW4" t="s">
+      <c r="AX4">
+        <v>5</v>
+      </c>
+      <c r="AY4" t="s">
         <v>90</v>
       </c>
-      <c r="AX4">
-        <v>5</v>
-      </c>
-      <c r="AY4" t="s">
+      <c r="AZ4">
+        <v>5</v>
+      </c>
+      <c r="BA4" t="s">
         <v>91</v>
       </c>
-      <c r="AZ4">
+      <c r="BB4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>914362579</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>42</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>3.5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>43</v>
       </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
         <v>44</v>
       </c>
-      <c r="H5">
-        <v>4.5</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J5">
+        <v>4.5</v>
+      </c>
+      <c r="K5" t="s">
         <v>45</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>8</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>46</v>
       </c>
-      <c r="L5">
-        <v>4</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5" t="s">
         <v>47</v>
       </c>
-      <c r="N5">
-        <v>4.5</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="P5">
+        <v>4.5</v>
+      </c>
+      <c r="Q5" t="s">
         <v>49</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>5.5</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>48</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>10</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>50</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>993152642</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>108</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>3.5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>109</v>
       </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
         <v>104</v>
       </c>
-      <c r="H6">
-        <v>4.5</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="J6">
+        <v>4.5</v>
+      </c>
+      <c r="K6" t="s">
         <v>111</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>8</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>105</v>
       </c>
-      <c r="L6">
-        <v>4</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6" t="s">
         <v>47</v>
       </c>
-      <c r="N6">
-        <v>4.5</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="P6">
+        <v>4.5</v>
+      </c>
+      <c r="Q6" t="s">
         <v>49</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>5.5</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>48</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>10</v>
       </c>
-      <c r="S6" t="s">
+      <c r="U6" t="s">
         <v>50</v>
       </c>
-      <c r="T6">
+      <c r="V6">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>963186254</v>
       </c>
@@ -1361,91 +1427,97 @@
         <v>51</v>
       </c>
       <c r="C7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" t="s">
         <v>52</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>110</v>
       </c>
       <c r="F7">
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="H7">
         <v>3</v>
       </c>
       <c r="I7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
         <v>55</v>
       </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7" t="s">
         <v>56</v>
       </c>
-      <c r="L7">
-        <v>5</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="O7" t="s">
         <v>57</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>3</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>58</v>
-      </c>
-      <c r="P7">
-        <v>6</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>59</v>
       </c>
       <c r="R7">
         <v>6</v>
       </c>
       <c r="S7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T7">
         <v>6</v>
       </c>
       <c r="U7" t="s">
+        <v>60</v>
+      </c>
+      <c r="V7">
+        <v>6</v>
+      </c>
+      <c r="W7" t="s">
         <v>61</v>
       </c>
-      <c r="V7">
-        <v>5</v>
-      </c>
-      <c r="W7" t="s">
+      <c r="X7">
+        <v>5</v>
+      </c>
+      <c r="Y7" t="s">
         <v>62</v>
-      </c>
-      <c r="X7">
-        <v>3</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>63</v>
       </c>
       <c r="Z7">
         <v>3</v>
       </c>
       <c r="AA7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB7">
+        <v>3</v>
+      </c>
+      <c r="AC7" t="s">
         <v>64</v>
       </c>
-      <c r="AB7">
+      <c r="AD7">
         <v>6</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AE7" t="s">
         <v>65</v>
       </c>
-      <c r="AD7">
+      <c r="AF7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>984521523</v>
       </c>
@@ -1453,157 +1525,163 @@
         <v>66</v>
       </c>
       <c r="C8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" t="s">
         <v>67</v>
       </c>
-      <c r="D8">
-        <v>4.5</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8">
+        <v>4.5</v>
+      </c>
+      <c r="G8" t="s">
         <v>68</v>
       </c>
-      <c r="F8">
-        <v>4.5</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8">
+        <v>4.5</v>
+      </c>
+      <c r="I8" t="s">
         <v>69</v>
       </c>
-      <c r="H8">
-        <v>4.5</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="J8">
+        <v>4.5</v>
+      </c>
+      <c r="K8" t="s">
         <v>70</v>
       </c>
-      <c r="J8">
-        <v>4.5</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="L8">
+        <v>4.5</v>
+      </c>
+      <c r="M8" t="s">
         <v>71</v>
       </c>
-      <c r="L8">
-        <v>4.5</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="N8">
+        <v>4.5</v>
+      </c>
+      <c r="O8" t="s">
         <v>72</v>
       </c>
-      <c r="N8">
-        <v>5</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="P8">
+        <v>5</v>
+      </c>
+      <c r="Q8" t="s">
         <v>73</v>
       </c>
-      <c r="P8">
-        <v>5</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="R8">
+        <v>5</v>
+      </c>
+      <c r="S8" t="s">
         <v>74</v>
       </c>
-      <c r="R8">
-        <v>4</v>
-      </c>
-      <c r="S8" t="s">
+      <c r="T8">
+        <v>4</v>
+      </c>
+      <c r="U8" t="s">
         <v>75</v>
       </c>
-      <c r="T8">
-        <v>4</v>
-      </c>
-      <c r="U8" t="s">
+      <c r="V8">
+        <v>4</v>
+      </c>
+      <c r="W8" t="s">
         <v>76</v>
       </c>
-      <c r="V8">
-        <v>4</v>
-      </c>
-      <c r="W8" t="s">
+      <c r="X8">
+        <v>4</v>
+      </c>
+      <c r="Y8" t="s">
         <v>77</v>
       </c>
-      <c r="X8">
-        <v>4</v>
-      </c>
-      <c r="Y8" t="s">
+      <c r="Z8">
+        <v>4</v>
+      </c>
+      <c r="AA8" t="s">
         <v>78</v>
       </c>
-      <c r="Z8">
-        <v>4</v>
-      </c>
-      <c r="AA8" t="s">
+      <c r="AB8">
+        <v>4</v>
+      </c>
+      <c r="AC8" t="s">
         <v>79</v>
       </c>
-      <c r="AB8">
-        <v>4.5</v>
-      </c>
-      <c r="AC8" t="s">
+      <c r="AD8">
+        <v>4.5</v>
+      </c>
+      <c r="AE8" t="s">
         <v>80</v>
       </c>
-      <c r="AD8">
-        <v>5</v>
-      </c>
-      <c r="AE8" t="s">
+      <c r="AF8">
+        <v>5</v>
+      </c>
+      <c r="AG8" t="s">
         <v>81</v>
       </c>
-      <c r="AF8">
-        <v>5</v>
-      </c>
-      <c r="AG8" t="s">
+      <c r="AH8">
+        <v>5</v>
+      </c>
+      <c r="AI8" t="s">
         <v>82</v>
       </c>
-      <c r="AH8">
-        <v>5</v>
-      </c>
-      <c r="AI8" t="s">
+      <c r="AJ8">
+        <v>5</v>
+      </c>
+      <c r="AK8" t="s">
         <v>83</v>
       </c>
-      <c r="AJ8">
-        <v>5</v>
-      </c>
-      <c r="AK8" t="s">
+      <c r="AL8">
+        <v>5</v>
+      </c>
+      <c r="AM8" t="s">
         <v>84</v>
       </c>
-      <c r="AL8">
-        <v>5</v>
-      </c>
-      <c r="AM8" t="s">
+      <c r="AN8">
+        <v>5</v>
+      </c>
+      <c r="AO8" t="s">
         <v>85</v>
       </c>
-      <c r="AN8">
-        <v>5</v>
-      </c>
-      <c r="AO8" t="s">
+      <c r="AP8">
+        <v>5</v>
+      </c>
+      <c r="AQ8" t="s">
         <v>86</v>
       </c>
-      <c r="AP8">
-        <v>5</v>
-      </c>
-      <c r="AQ8" t="s">
+      <c r="AR8">
+        <v>5</v>
+      </c>
+      <c r="AS8" t="s">
         <v>87</v>
       </c>
-      <c r="AR8">
-        <v>5</v>
-      </c>
-      <c r="AS8" t="s">
+      <c r="AT8">
+        <v>5</v>
+      </c>
+      <c r="AU8" t="s">
         <v>88</v>
       </c>
-      <c r="AT8">
-        <v>5</v>
-      </c>
-      <c r="AU8" t="s">
+      <c r="AV8">
+        <v>5</v>
+      </c>
+      <c r="AW8" t="s">
         <v>89</v>
       </c>
-      <c r="AV8">
-        <v>5</v>
-      </c>
-      <c r="AW8" t="s">
+      <c r="AX8">
+        <v>5</v>
+      </c>
+      <c r="AY8" t="s">
         <v>90</v>
       </c>
-      <c r="AX8">
-        <v>5</v>
-      </c>
-      <c r="AY8" t="s">
+      <c r="AZ8">
+        <v>5</v>
+      </c>
+      <c r="BA8" t="s">
         <v>91</v>
       </c>
-      <c r="AZ8">
+      <c r="BB8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>995148632</v>
       </c>
@@ -1611,91 +1689,97 @@
         <v>51</v>
       </c>
       <c r="C9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" t="s">
         <v>52</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>53</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H9">
         <v>3</v>
       </c>
       <c r="I9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9" t="s">
         <v>55</v>
       </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9" t="s">
         <v>56</v>
       </c>
-      <c r="L9">
-        <v>5</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="N9">
+        <v>5</v>
+      </c>
+      <c r="O9" t="s">
         <v>57</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>3</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>58</v>
-      </c>
-      <c r="P9">
-        <v>6</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>59</v>
       </c>
       <c r="R9">
         <v>6</v>
       </c>
       <c r="S9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T9">
         <v>6</v>
       </c>
       <c r="U9" t="s">
+        <v>60</v>
+      </c>
+      <c r="V9">
+        <v>6</v>
+      </c>
+      <c r="W9" t="s">
         <v>61</v>
       </c>
-      <c r="V9">
-        <v>5</v>
-      </c>
-      <c r="W9" t="s">
+      <c r="X9">
+        <v>5</v>
+      </c>
+      <c r="Y9" t="s">
         <v>62</v>
-      </c>
-      <c r="X9">
-        <v>3</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>63</v>
       </c>
       <c r="Z9">
         <v>3</v>
       </c>
       <c r="AA9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB9">
+        <v>3</v>
+      </c>
+      <c r="AC9" t="s">
         <v>64</v>
       </c>
-      <c r="AB9">
+      <c r="AD9">
         <v>6</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AE9" t="s">
         <v>65</v>
       </c>
-      <c r="AD9">
+      <c r="AF9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>912375486</v>
       </c>
@@ -1703,157 +1787,168 @@
         <v>66</v>
       </c>
       <c r="C10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" t="s">
         <v>67</v>
       </c>
-      <c r="D10">
-        <v>4.5</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10">
+        <v>4.5</v>
+      </c>
+      <c r="G10" t="s">
         <v>68</v>
       </c>
-      <c r="F10">
-        <v>4.5</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="H10">
+        <v>4.5</v>
+      </c>
+      <c r="I10" t="s">
         <v>107</v>
       </c>
-      <c r="H10">
-        <v>4.5</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="J10">
+        <v>4.5</v>
+      </c>
+      <c r="K10" t="s">
         <v>70</v>
       </c>
-      <c r="J10">
-        <v>4.5</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="L10">
+        <v>4.5</v>
+      </c>
+      <c r="M10" t="s">
         <v>71</v>
       </c>
-      <c r="L10">
-        <v>4.5</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="N10">
+        <v>4.5</v>
+      </c>
+      <c r="O10" t="s">
         <v>72</v>
       </c>
-      <c r="N10">
-        <v>5</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="P10">
+        <v>5</v>
+      </c>
+      <c r="Q10" t="s">
         <v>73</v>
       </c>
-      <c r="P10">
-        <v>5</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="R10">
+        <v>5</v>
+      </c>
+      <c r="S10" t="s">
         <v>74</v>
       </c>
-      <c r="R10">
-        <v>4</v>
-      </c>
-      <c r="S10" t="s">
+      <c r="T10">
+        <v>4</v>
+      </c>
+      <c r="U10" t="s">
         <v>75</v>
       </c>
-      <c r="T10">
-        <v>4</v>
-      </c>
-      <c r="U10" t="s">
+      <c r="V10">
+        <v>4</v>
+      </c>
+      <c r="W10" t="s">
         <v>76</v>
       </c>
-      <c r="V10">
-        <v>4</v>
-      </c>
-      <c r="W10" t="s">
+      <c r="X10">
+        <v>4</v>
+      </c>
+      <c r="Y10" t="s">
         <v>77</v>
       </c>
-      <c r="X10">
-        <v>4</v>
-      </c>
-      <c r="Y10" t="s">
+      <c r="Z10">
+        <v>4</v>
+      </c>
+      <c r="AA10" t="s">
         <v>78</v>
       </c>
-      <c r="Z10">
-        <v>4</v>
-      </c>
-      <c r="AA10" t="s">
+      <c r="AB10">
+        <v>4</v>
+      </c>
+      <c r="AC10" t="s">
         <v>79</v>
       </c>
-      <c r="AB10">
-        <v>4.5</v>
-      </c>
-      <c r="AC10" t="s">
+      <c r="AD10">
+        <v>4.5</v>
+      </c>
+      <c r="AE10" t="s">
         <v>80</v>
       </c>
-      <c r="AD10">
-        <v>5</v>
-      </c>
-      <c r="AE10" t="s">
+      <c r="AF10">
+        <v>5</v>
+      </c>
+      <c r="AG10" t="s">
         <v>81</v>
       </c>
-      <c r="AF10">
-        <v>5</v>
-      </c>
-      <c r="AG10" t="s">
+      <c r="AH10">
+        <v>5</v>
+      </c>
+      <c r="AI10" t="s">
         <v>82</v>
       </c>
-      <c r="AH10">
-        <v>5</v>
-      </c>
-      <c r="AI10" t="s">
+      <c r="AJ10">
+        <v>5</v>
+      </c>
+      <c r="AK10" t="s">
         <v>83</v>
       </c>
-      <c r="AJ10">
-        <v>5</v>
-      </c>
-      <c r="AK10" t="s">
+      <c r="AL10">
+        <v>5</v>
+      </c>
+      <c r="AM10" t="s">
         <v>84</v>
       </c>
-      <c r="AL10">
-        <v>5</v>
-      </c>
-      <c r="AM10" t="s">
+      <c r="AN10">
+        <v>5</v>
+      </c>
+      <c r="AO10" t="s">
         <v>85</v>
       </c>
-      <c r="AN10">
-        <v>5</v>
-      </c>
-      <c r="AO10" t="s">
+      <c r="AP10">
+        <v>5</v>
+      </c>
+      <c r="AQ10" t="s">
         <v>86</v>
       </c>
-      <c r="AP10">
-        <v>5</v>
-      </c>
-      <c r="AQ10" t="s">
+      <c r="AR10">
+        <v>5</v>
+      </c>
+      <c r="AS10" t="s">
         <v>87</v>
       </c>
-      <c r="AR10">
-        <v>5</v>
-      </c>
-      <c r="AS10" t="s">
+      <c r="AT10">
+        <v>5</v>
+      </c>
+      <c r="AU10" t="s">
         <v>88</v>
       </c>
-      <c r="AT10">
-        <v>5</v>
-      </c>
-      <c r="AU10" t="s">
+      <c r="AV10">
+        <v>5</v>
+      </c>
+      <c r="AW10" t="s">
         <v>89</v>
       </c>
-      <c r="AV10">
-        <v>5</v>
-      </c>
-      <c r="AW10" t="s">
+      <c r="AX10">
+        <v>5</v>
+      </c>
+      <c r="AY10" t="s">
         <v>90</v>
       </c>
-      <c r="AX10">
-        <v>5</v>
-      </c>
-      <c r="AY10" t="s">
+      <c r="AZ10">
+        <v>5</v>
+      </c>
+      <c r="BA10" t="s">
         <v>91</v>
       </c>
-      <c r="AZ10">
+      <c r="BB10">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2"/>
+    <hyperlink ref="D10" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1864,7 +1959,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1876,7 +1971,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>